<commit_message>
Updated files after Bayesian Inference
</commit_message>
<xml_diff>
--- a/ExcelFiles/failureProbabilities.xlsx
+++ b/ExcelFiles/failureProbabilities.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eslack/Documents/Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eslack/Documents/Code/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2CDD9C-F15E-6D46-9557-DF3B8028BFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A064687E-44F1-E04E-8695-034945188E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39020" yWindow="4280" windowWidth="32060" windowHeight="18540" activeTab="2" xr2:uid="{C3538AC8-E899-2A47-BF41-04CCB9B459B4}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="30240" windowHeight="17180" activeTab="2" xr2:uid="{C3538AC8-E899-2A47-BF41-04CCB9B459B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Table from CoreWind" sheetId="1" r:id="rId1"/>
     <sheet name="Pairing Failure Modes &amp; Effects" sheetId="3" r:id="rId2"/>
     <sheet name="Conditional Probabilities" sheetId="4" r:id="rId3"/>
+    <sheet name="Conditional Probabilities (2)" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="205">
   <si>
     <t>Component</t>
   </si>
@@ -359,13 +360,311 @@
   </si>
   <si>
     <t>Excessive load on cable</t>
+  </si>
+  <si>
+    <t>Incorrect turbine operation 1</t>
+  </si>
+  <si>
+    <t>Increased turbine loads/acceleration 1</t>
+  </si>
+  <si>
+    <t>Vessel or aircraft collision 1</t>
+  </si>
+  <si>
+    <t>Falling topside components 1</t>
+  </si>
+  <si>
+    <t>Turbine parked 1</t>
+  </si>
+  <si>
+    <t>Reduced power output 1</t>
+  </si>
+  <si>
+    <t>Drift off station 1</t>
+  </si>
+  <si>
+    <t>Compromised buoyancy/stability 1</t>
+  </si>
+  <si>
+    <t>Large hydrostatic offset (angle of list/loll or draft change) 1</t>
+  </si>
+  <si>
+    <t>Excess dynamics 1</t>
+  </si>
+  <si>
+    <t>Capsize 1</t>
+  </si>
+  <si>
+    <t>Sink 1</t>
+  </si>
+  <si>
+    <t>Mooring-mooring clashing - 1</t>
+  </si>
+  <si>
+    <t>Mooring-cable clashing - 1</t>
+  </si>
+  <si>
+    <t>Anchor-cable clashing - 1</t>
+  </si>
+  <si>
+    <t>Change in mooring profile - a</t>
+  </si>
+  <si>
+    <t>Change in mooring profile - b</t>
+  </si>
+  <si>
+    <t>Excess mooring loads - a</t>
+  </si>
+  <si>
+    <t>Excess mooring loads - b</t>
+  </si>
+  <si>
+    <t>Mooring line nonfunctional - a</t>
+  </si>
+  <si>
+    <t>Mooring line nonfunctional - b</t>
+  </si>
+  <si>
+    <t>Excess anchor load - a</t>
+  </si>
+  <si>
+    <t>Excess anchor load - b</t>
+  </si>
+  <si>
+    <t>Anchor dragging - a</t>
+  </si>
+  <si>
+    <t>Anchor dragging - b</t>
+  </si>
+  <si>
+    <t>Array cable: Loss of connectivity 1</t>
+  </si>
+  <si>
+    <t>RNA structural 1</t>
+  </si>
+  <si>
+    <t>generator &amp; gearbox 1</t>
+  </si>
+  <si>
+    <t>turbine controls 1</t>
+  </si>
+  <si>
+    <t>tower structural 1</t>
+  </si>
+  <si>
+    <t>platform (structural integrity) 1</t>
+  </si>
+  <si>
+    <t>platform (watertightness) 1</t>
+  </si>
+  <si>
+    <t>ballast system failure 1</t>
+  </si>
+  <si>
+    <t>chain 1a</t>
+  </si>
+  <si>
+    <t>chain 1b</t>
+  </si>
+  <si>
+    <t>synthetic rope 1a</t>
+  </si>
+  <si>
+    <t>synthetic rope 1b</t>
+  </si>
+  <si>
+    <t>single anchor 1a</t>
+  </si>
+  <si>
+    <t>single anchor 1b</t>
+  </si>
+  <si>
+    <t>Incorrect turbine operation 2</t>
+  </si>
+  <si>
+    <t>Increased turbine loads/acceleration 2</t>
+  </si>
+  <si>
+    <t>Vessel or aircraft collision 2</t>
+  </si>
+  <si>
+    <t>Falling topside components 2</t>
+  </si>
+  <si>
+    <t>Turbine parked 2</t>
+  </si>
+  <si>
+    <t>Reduced power output 2</t>
+  </si>
+  <si>
+    <t>Drift off station 2</t>
+  </si>
+  <si>
+    <t>Compromised buoyancy/stability 2</t>
+  </si>
+  <si>
+    <t>Large hydrostatic offset (angle of list/loll or draft change) 2</t>
+  </si>
+  <si>
+    <t>Excess dynamics 2</t>
+  </si>
+  <si>
+    <t>Capsize 2</t>
+  </si>
+  <si>
+    <t>Sink 2</t>
+  </si>
+  <si>
+    <t>Mooring-mooring clashing - 2</t>
+  </si>
+  <si>
+    <t>Mooring-cable clashing - 2n</t>
+  </si>
+  <si>
+    <t>Mooring-cable clashing - 2m</t>
+  </si>
+  <si>
+    <t>Anchor-cable clashing - 2n</t>
+  </si>
+  <si>
+    <t>Anchor-cable clashing - 2m</t>
+  </si>
+  <si>
+    <t>Change in mooring profile - c</t>
+  </si>
+  <si>
+    <t>Change in mooring profile - d</t>
+  </si>
+  <si>
+    <t>Excess mooring loads - c</t>
+  </si>
+  <si>
+    <t>Excess mooring loads - d</t>
+  </si>
+  <si>
+    <t>Mooring line nonfunctional - c</t>
+  </si>
+  <si>
+    <t>Mooring line nonfunctional - d</t>
+  </si>
+  <si>
+    <t>Excess anchor load - c</t>
+  </si>
+  <si>
+    <t>Excess anchor load - d</t>
+  </si>
+  <si>
+    <t>Anchor dragging - c</t>
+  </si>
+  <si>
+    <t>Anchor dragging - d</t>
+  </si>
+  <si>
+    <t>Array cable: Loss of connectivity 2n</t>
+  </si>
+  <si>
+    <t>Array cable: Loss of connectivity 2m</t>
+  </si>
+  <si>
+    <t>RNA structural 2</t>
+  </si>
+  <si>
+    <t>generator &amp; gearbox 2</t>
+  </si>
+  <si>
+    <t>turbine controls 2</t>
+  </si>
+  <si>
+    <t>tower structural 2</t>
+  </si>
+  <si>
+    <t>platform (structural integrity) 2</t>
+  </si>
+  <si>
+    <t>platform (watertightness) 2</t>
+  </si>
+  <si>
+    <t>ballast system failure 2</t>
+  </si>
+  <si>
+    <t>chain 2c</t>
+  </si>
+  <si>
+    <t>chain 2d</t>
+  </si>
+  <si>
+    <t>synthetic rope 2c</t>
+  </si>
+  <si>
+    <t>synthetic rope 2d</t>
+  </si>
+  <si>
+    <t>single anchor 2c</t>
+  </si>
+  <si>
+    <t>single anchor 2d</t>
+  </si>
+  <si>
+    <t>Shared line nonfunctional - s</t>
+  </si>
+  <si>
+    <t>Mooring-cable clashing - sn</t>
+  </si>
+  <si>
+    <t>Change in cable profile - n</t>
+  </si>
+  <si>
+    <t>Change in cable profile - m</t>
+  </si>
+  <si>
+    <t>Excessive load on cable - n</t>
+  </si>
+  <si>
+    <t>Excessive load on cable - m</t>
+  </si>
+  <si>
+    <t>Substation/grid interruption - B</t>
+  </si>
+  <si>
+    <t>Reduced AEP - B</t>
+  </si>
+  <si>
+    <t>chain - s</t>
+  </si>
+  <si>
+    <t>clump weights or floats - s</t>
+  </si>
+  <si>
+    <t>tether and anchor systems - B</t>
+  </si>
+  <si>
+    <t>cable protection system - B</t>
+  </si>
+  <si>
+    <t>dynamic cable - n</t>
+  </si>
+  <si>
+    <t>dynamic cable - m</t>
+  </si>
+  <si>
+    <t>static cable - m</t>
+  </si>
+  <si>
+    <t>terminations - B</t>
+  </si>
+  <si>
+    <t>offshore joints - B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="174" formatCode="_(* #,##0.0000000000000_);_(* \(#,##0.0000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -386,8 +685,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,6 +751,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF6F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDFEDFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7FFF2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFDA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2EBFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE8EF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -981,10 +1317,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1331,11 +1668,102 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1347,10 +1775,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFE4F6FF"/>
+      <color rgb="FFFFE8EF"/>
+      <color rgb="FFF2EBFF"/>
+      <color rgb="FFFFFFDA"/>
       <color rgb="FFF7FFF2"/>
       <color rgb="FFFFF6F0"/>
       <color rgb="FFDFEDFF"/>
+      <color rgb="FFE4F6FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2973,7 +3404,7 @@
     <mergeCell ref="I21:I22"/>
   </mergeCells>
   <conditionalFormatting sqref="I4:K31">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="1">
       <formula>LEN(TRIM(I4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2985,8 +3416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FCDD4F1-A2BC-0B42-962A-C68F52B3972A}">
   <dimension ref="A3:AE63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="292" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AD10" sqref="AD10"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="156" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B51" sqref="B5:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3103,7 +3534,7 @@
         <v>1.95E-2</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="99" t="s">
         <v>54</v>
@@ -3299,7 +3730,7 @@
         <v>1.3625E-2</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="102" t="s">
         <v>54</v>
@@ -3392,7 +3823,7 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8" s="102" t="s">
         <v>54</v>
@@ -3461,7 +3892,7 @@
         <v>1.7499999999999998E-2</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E9" s="102" t="s">
         <v>54</v>
@@ -3529,6 +3960,9 @@
         <f>'Pairing Failure Modes &amp; Effects'!H6</f>
         <v>0.20750000000000002</v>
       </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
       <c r="E10" s="102" t="s">
         <v>54</v>
       </c>
@@ -3596,7 +4030,7 @@
         <v>1E-3</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E11" s="103" t="s">
         <v>54</v>
@@ -3665,7 +4099,7 @@
         <v>1E-3</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E12" s="45" t="s">
         <v>55</v>
@@ -3734,7 +4168,7 @@
         <v>1E-3</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E13" s="45" t="s">
         <v>55</v>
@@ -3803,7 +4237,7 @@
         <v>9.3185000000000004E-2</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E14" s="45" t="s">
         <v>55</v>
@@ -3872,7 +4306,7 @@
         <v>1E-3</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E15" s="45" t="s">
         <v>55</v>
@@ -3941,7 +4375,7 @@
         <v>1E-3</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E16" s="45" t="s">
         <v>55</v>
@@ -4010,7 +4444,7 @@
         <v>2.73109375E-2</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E17" s="45" t="s">
         <v>55</v>
@@ -4079,7 +4513,7 @@
         <v>3.3968125000000002E-2</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E18" s="45" t="s">
         <v>55</v>
@@ -4148,7 +4582,7 @@
         <v>3.3968125000000002E-2</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E19" s="45" t="s">
         <v>83</v>
@@ -4217,7 +4651,7 @@
         <v>1.375E-2</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E20" s="45" t="s">
         <v>83</v>
@@ -4286,7 +4720,7 @@
         <v>1.375E-2</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E21" s="45" t="s">
         <v>83</v>
@@ -4355,7 +4789,7 @@
         <v>1.375E-2</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E22" s="45" t="s">
         <v>83</v>
@@ -4424,7 +4858,7 @@
         <v>1.375E-2</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E23" s="45" t="s">
         <v>83</v>
@@ -4493,7 +4927,7 @@
         <v>1.375E-2</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E24" s="45" t="s">
         <v>83</v>
@@ -4562,7 +4996,7 @@
         <v>1.375E-2</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E25" s="45" t="s">
         <v>83</v>
@@ -4631,7 +5065,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E26" s="45" t="s">
         <v>83</v>
@@ -4700,7 +5134,7 @@
         <v>2.0500000000000001E-2</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E27" s="45" t="s">
         <v>83</v>
@@ -4769,7 +5203,7 @@
         <v>0.02</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="E28" s="45" t="s">
         <v>83</v>
@@ -4838,7 +5272,7 @@
         <v>0.01</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E29" s="45" t="s">
         <v>83</v>
@@ -4906,6 +5340,9 @@
         <f>'Pairing Failure Modes &amp; Effects'!H31</f>
         <v>0.01</v>
       </c>
+      <c r="D30">
+        <v>25</v>
+      </c>
       <c r="E30" s="45" t="s">
         <v>83</v>
       </c>
@@ -4973,7 +5410,7 @@
         <v>0.23300000000000001</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="E31" s="45" t="s">
         <v>83</v>
@@ -5042,7 +5479,7 @@
         <v>0.28800000000000003</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="E32" s="45" t="s">
         <v>83</v>
@@ -5111,7 +5548,7 @@
         <v>0.54337399999999991</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="E33" s="45" t="s">
         <v>83</v>
@@ -5180,7 +5617,7 @@
         <v>0.1285</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="E34" s="45" t="s">
         <v>83</v>
@@ -5249,7 +5686,7 @@
         <v>0.01</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E35" s="45" t="s">
         <v>83</v>
@@ -5318,7 +5755,7 @@
         <v>0.01</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E36" s="45" t="s">
         <v>83</v>
@@ -5387,7 +5824,7 @@
         <v>0.01</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E37" s="45" t="s">
         <v>83</v>
@@ -5456,7 +5893,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="E38" s="45" t="s">
         <v>83</v>
@@ -5525,7 +5962,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="E39" s="45" t="s">
         <v>83</v>
@@ -5594,7 +6031,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="E40" s="45" t="s">
         <v>83</v>
@@ -5663,7 +6100,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="E41" s="45" t="s">
         <v>83</v>
@@ -5732,7 +6169,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="E42" s="45" t="s">
         <v>83</v>
@@ -5801,7 +6238,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="E43" s="45" t="s">
         <v>79</v>
@@ -5870,7 +6307,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="E44" s="45" t="s">
         <v>79</v>
@@ -5938,7 +6375,7 @@
         <v>0.33</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="E45" s="45" t="s">
         <v>79</v>
@@ -6006,7 +6443,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="E46" s="45" t="s">
         <v>79</v>
@@ -6074,7 +6511,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="E47" s="45" t="s">
         <v>79</v>
@@ -6142,7 +6579,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="E48" s="45" t="s">
         <v>79</v>
@@ -6210,7 +6647,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="E49" s="45" t="s">
         <v>79</v>
@@ -6278,7 +6715,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="E50" s="45" t="s">
         <v>79</v>
@@ -6346,7 +6783,7 @@
         <v>0.10500000000000001</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="E51" s="45" t="s">
         <v>79</v>
@@ -6430,6 +6867,10 @@
       </c>
     </row>
     <row r="53" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="B53" s="137">
+        <f>(9*47+D49)/470</f>
+        <v>0.99361702127659579</v>
+      </c>
       <c r="E53" s="45" t="s">
         <v>79</v>
       </c>
@@ -6649,6 +7090,1326 @@
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="E62:K63"/>
   </mergeCells>
+  <conditionalFormatting sqref="C5:C30">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31:C51">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+      <formula>0.01</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+      <formula>"0..01"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B23A20A-06BD-C94D-947C-C47B31E9A88E}">
+  <dimension ref="A2:AE99"/>
+  <sheetViews>
+    <sheetView zoomScale="89" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="42.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="7" max="7" width="31.83203125" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
+    <col min="9" max="9" width="30.5" customWidth="1"/>
+    <col min="10" max="11" width="20.5" customWidth="1"/>
+    <col min="17" max="17" width="31.1640625" customWidth="1"/>
+    <col min="19" max="19" width="15.33203125" customWidth="1"/>
+    <col min="20" max="20" width="12" customWidth="1"/>
+    <col min="21" max="21" width="12.1640625" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" customWidth="1"/>
+    <col min="28" max="28" width="12.5" customWidth="1"/>
+    <col min="29" max="29" width="12.6640625" customWidth="1"/>
+    <col min="30" max="30" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="125" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="121">
+        <v>1.95E-2</v>
+      </c>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+    </row>
+    <row r="3" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="126" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="121">
+        <v>1.95E-2</v>
+      </c>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+    </row>
+    <row r="4" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="126" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="120">
+        <v>1.3625E-2</v>
+      </c>
+      <c r="D4" s="120"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="120"/>
+    </row>
+    <row r="5" spans="1:31" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="126" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="120">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="D5" s="120"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="120"/>
+      <c r="H5" s="120"/>
+      <c r="I5" s="120"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="Y5" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>104</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="126" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="120">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="D6" s="120"/>
+      <c r="K6" s="121"/>
+      <c r="L6" s="120"/>
+      <c r="Q6" s="45"/>
+      <c r="Y6" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z6">
+        <f>C39</f>
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <f>C22</f>
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <f>Z6*AA6</f>
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <f>MIN(Z6:AA6)</f>
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <f>(AB6+AC6)/2 *AA6</f>
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <f>1-AD6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="126" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="120">
+        <v>0.20749999999999999</v>
+      </c>
+      <c r="D7" s="120"/>
+      <c r="K7" s="120"/>
+      <c r="L7" s="120"/>
+      <c r="Q7" s="45"/>
+      <c r="Y7" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z7">
+        <f>C41</f>
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <f>AA6</f>
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <f>Z7*AA7</f>
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <f>MIN(Z7:AA7)</f>
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <f>(AB7+AC7)/2 *AA7</f>
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <f>1-AD7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="127" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="122">
+        <v>1E-3</v>
+      </c>
+      <c r="D8" s="120"/>
+      <c r="K8" s="120"/>
+      <c r="L8" s="120"/>
+      <c r="Q8" s="45"/>
+      <c r="Z8">
+        <f>1-Z6</f>
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <f>AA7</f>
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <f>Z8*AA8</f>
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <f>MIN(Z8:AA8)</f>
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <f>(AB8+AC8)/2 *AA8</f>
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <f>1-AD8</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="128" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="136">
+        <v>1E-3</v>
+      </c>
+      <c r="D9" s="120"/>
+      <c r="K9" s="120"/>
+      <c r="L9" s="120"/>
+      <c r="Q9" s="45"/>
+    </row>
+    <row r="10" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="128" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="136">
+        <v>1E-3</v>
+      </c>
+      <c r="D10" s="120"/>
+      <c r="K10" s="120"/>
+      <c r="L10" s="120"/>
+      <c r="Q10" s="45"/>
+    </row>
+    <row r="11" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="128" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="136">
+        <v>9.3185000000000004E-2</v>
+      </c>
+      <c r="D11" s="120"/>
+      <c r="K11" s="120"/>
+      <c r="L11" s="120"/>
+      <c r="Q11" s="45"/>
+    </row>
+    <row r="12" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="128" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="136">
+        <v>1E-3</v>
+      </c>
+      <c r="D12" s="120"/>
+      <c r="K12" s="122"/>
+      <c r="L12" s="120"/>
+      <c r="Q12" s="45"/>
+    </row>
+    <row r="13" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="128" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="136">
+        <v>1E-3</v>
+      </c>
+      <c r="D13" s="120"/>
+      <c r="K13" s="120"/>
+      <c r="L13" s="120"/>
+      <c r="Q13" s="45"/>
+    </row>
+    <row r="14" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="128" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="136">
+        <v>2.7310938E-2</v>
+      </c>
+      <c r="D14" s="120"/>
+      <c r="K14" s="120"/>
+      <c r="L14" s="120"/>
+      <c r="Q14" s="45"/>
+    </row>
+    <row r="15" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="128" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="136">
+        <v>3.3969125000000003E-2</v>
+      </c>
+      <c r="D15" s="120"/>
+      <c r="K15" s="120"/>
+      <c r="L15" s="120"/>
+      <c r="Q15" s="45"/>
+    </row>
+    <row r="16" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="128" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="136">
+        <v>3.3969125000000003E-2</v>
+      </c>
+      <c r="D16" s="120"/>
+      <c r="K16" s="120"/>
+      <c r="L16" s="120"/>
+      <c r="Q16" s="45"/>
+    </row>
+    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="128" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D17" s="120"/>
+      <c r="K17" s="120"/>
+      <c r="L17" s="120"/>
+      <c r="Q17" s="45"/>
+    </row>
+    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="128" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D18" s="120"/>
+      <c r="K18" s="120"/>
+      <c r="L18" s="120"/>
+      <c r="Q18" s="45"/>
+    </row>
+    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="128" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D19" s="120"/>
+      <c r="K19" s="120"/>
+      <c r="L19" s="120"/>
+      <c r="Q19" s="45"/>
+    </row>
+    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="128" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D20" s="120"/>
+      <c r="K20" s="120"/>
+      <c r="L20" s="120"/>
+      <c r="Q20" s="45"/>
+    </row>
+    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="128" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D21" s="120"/>
+      <c r="K21" s="120"/>
+      <c r="L21" s="120"/>
+      <c r="Q21" s="45"/>
+    </row>
+    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="128" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D22" s="120"/>
+      <c r="K22" s="120"/>
+      <c r="L22" s="120"/>
+      <c r="Q22" s="45"/>
+    </row>
+    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="128" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D23" s="120"/>
+      <c r="I23" s="121"/>
+      <c r="J23" s="120"/>
+      <c r="K23" s="120"/>
+      <c r="L23" s="120"/>
+      <c r="Q23" s="45"/>
+    </row>
+    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="128" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D24" s="120"/>
+      <c r="I24" s="121"/>
+      <c r="J24" s="120"/>
+      <c r="K24" s="120"/>
+      <c r="L24" s="120"/>
+      <c r="Q24" s="45"/>
+    </row>
+    <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="128" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D25" s="120"/>
+      <c r="I25" s="121"/>
+      <c r="J25" s="120"/>
+      <c r="K25" s="120"/>
+      <c r="L25" s="120"/>
+      <c r="Q25" s="45"/>
+    </row>
+    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="128" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D26" s="120"/>
+      <c r="I26" s="121"/>
+      <c r="J26" s="120"/>
+      <c r="K26" s="120"/>
+      <c r="L26" s="120"/>
+      <c r="Q26" s="45"/>
+    </row>
+    <row r="27" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="128" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" s="136">
+        <v>0.02</v>
+      </c>
+      <c r="D27" s="120"/>
+      <c r="I27" s="121"/>
+      <c r="J27" s="120"/>
+      <c r="K27" s="120"/>
+      <c r="L27" s="120"/>
+      <c r="Q27" s="45"/>
+    </row>
+    <row r="28" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="129" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" s="136">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="D28" s="120"/>
+      <c r="I28" s="121"/>
+      <c r="J28" s="120"/>
+      <c r="K28" s="120"/>
+      <c r="L28" s="120"/>
+      <c r="Q28" s="45"/>
+    </row>
+    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="129" t="s">
+        <v>134</v>
+      </c>
+      <c r="B29" s="136">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="D29" s="120"/>
+      <c r="I29" s="121"/>
+      <c r="J29" s="120"/>
+      <c r="K29" s="120"/>
+      <c r="L29" s="120"/>
+      <c r="Q29" s="45"/>
+    </row>
+    <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="129" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" s="136">
+        <v>0.54337400000000002</v>
+      </c>
+      <c r="D30" s="120"/>
+      <c r="I30" s="121"/>
+      <c r="J30" s="120"/>
+      <c r="K30" s="120"/>
+      <c r="L30" s="120"/>
+      <c r="Q30" s="45"/>
+    </row>
+    <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="129" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31" s="136">
+        <v>0.1285</v>
+      </c>
+      <c r="D31" s="120"/>
+      <c r="I31" s="121"/>
+      <c r="J31" s="120"/>
+      <c r="K31" s="120"/>
+      <c r="L31" s="120"/>
+      <c r="Q31" s="45"/>
+    </row>
+    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="129" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" s="136">
+        <v>0.01</v>
+      </c>
+      <c r="D32" s="120"/>
+      <c r="I32" s="121"/>
+      <c r="J32" s="120"/>
+      <c r="K32" s="120"/>
+      <c r="L32" s="120"/>
+      <c r="Q32" s="46"/>
+    </row>
+    <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="129" t="s">
+        <v>138</v>
+      </c>
+      <c r="B33" s="136">
+        <v>0.01</v>
+      </c>
+      <c r="D33" s="120"/>
+      <c r="I33" s="121"/>
+      <c r="J33" s="120"/>
+      <c r="K33" s="120"/>
+      <c r="L33" s="120"/>
+      <c r="Q33" s="46"/>
+    </row>
+    <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="129" t="s">
+        <v>139</v>
+      </c>
+      <c r="B34" s="136">
+        <v>0.01</v>
+      </c>
+      <c r="D34" s="120"/>
+      <c r="I34" s="121"/>
+      <c r="J34" s="120"/>
+      <c r="K34" s="120"/>
+      <c r="L34" s="120"/>
+      <c r="Q34" s="46"/>
+    </row>
+    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="129" t="s">
+        <v>140</v>
+      </c>
+      <c r="B35" s="136">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D35" s="120"/>
+      <c r="I35" s="121"/>
+      <c r="J35" s="120"/>
+      <c r="K35" s="120"/>
+      <c r="L35" s="120"/>
+      <c r="Q35" s="46"/>
+    </row>
+    <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="129" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="136">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D36" s="120"/>
+      <c r="I36" s="121"/>
+      <c r="J36" s="120"/>
+      <c r="K36" s="120"/>
+      <c r="L36" s="120"/>
+      <c r="Q36" s="46"/>
+    </row>
+    <row r="37" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="129" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="136">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D37" s="120"/>
+      <c r="I37" s="121"/>
+      <c r="J37" s="120"/>
+      <c r="K37" s="120"/>
+      <c r="L37" s="120"/>
+      <c r="Q37" s="46"/>
+    </row>
+    <row r="38" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="129" t="s">
+        <v>143</v>
+      </c>
+      <c r="B38" s="136">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D38" s="120"/>
+      <c r="I38" s="121"/>
+      <c r="J38" s="120"/>
+      <c r="K38" s="120"/>
+      <c r="L38" s="120"/>
+      <c r="Q38" s="46"/>
+    </row>
+    <row r="39" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="129" t="s">
+        <v>144</v>
+      </c>
+      <c r="B39" s="136">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D39" s="120"/>
+      <c r="I39" s="121"/>
+      <c r="J39" s="120"/>
+      <c r="K39" s="120"/>
+      <c r="L39" s="120"/>
+      <c r="Q39" s="46"/>
+    </row>
+    <row r="40" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="129" t="s">
+        <v>145</v>
+      </c>
+      <c r="B40" s="136">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D40" s="120"/>
+      <c r="I40" s="121"/>
+      <c r="J40" s="120"/>
+      <c r="K40" s="120"/>
+      <c r="L40" s="120"/>
+      <c r="Q40" s="46"/>
+    </row>
+    <row r="41" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="130" t="s">
+        <v>146</v>
+      </c>
+      <c r="B41" s="121">
+        <v>1.95E-2</v>
+      </c>
+      <c r="D41" s="120"/>
+      <c r="I41" s="121"/>
+      <c r="J41" s="120"/>
+      <c r="K41" s="120"/>
+      <c r="L41" s="120"/>
+      <c r="Q41" s="46"/>
+    </row>
+    <row r="42" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="130" t="s">
+        <v>147</v>
+      </c>
+      <c r="B42" s="121">
+        <v>1.95E-2</v>
+      </c>
+      <c r="D42" s="120"/>
+      <c r="I42" s="121"/>
+      <c r="J42" s="120"/>
+      <c r="K42" s="120"/>
+      <c r="L42" s="120"/>
+      <c r="Q42" s="46"/>
+    </row>
+    <row r="43" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="130" t="s">
+        <v>148</v>
+      </c>
+      <c r="B43" s="120">
+        <v>1.3625E-2</v>
+      </c>
+      <c r="D43" s="120"/>
+      <c r="I43" s="121"/>
+      <c r="J43" s="120"/>
+      <c r="K43" s="120"/>
+      <c r="L43" s="120"/>
+      <c r="Q43" s="46"/>
+    </row>
+    <row r="44" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="130" t="s">
+        <v>149</v>
+      </c>
+      <c r="B44" s="120">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="D44" s="120"/>
+      <c r="I44" s="121"/>
+      <c r="J44" s="120"/>
+      <c r="K44" s="120"/>
+      <c r="L44" s="120"/>
+      <c r="Q44" s="46"/>
+    </row>
+    <row r="45" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="130" t="s">
+        <v>150</v>
+      </c>
+      <c r="B45" s="120">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="D45" s="120"/>
+      <c r="I45" s="121"/>
+      <c r="J45" s="120"/>
+      <c r="K45" s="120"/>
+      <c r="L45" s="120"/>
+      <c r="Q45" s="46"/>
+    </row>
+    <row r="46" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="130" t="s">
+        <v>151</v>
+      </c>
+      <c r="B46" s="120">
+        <v>0.20749999999999999</v>
+      </c>
+      <c r="D46" s="120"/>
+      <c r="I46" s="121"/>
+      <c r="J46" s="120"/>
+      <c r="K46" s="120"/>
+      <c r="L46" s="120"/>
+      <c r="Q46" s="46"/>
+    </row>
+    <row r="47" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="130" t="s">
+        <v>152</v>
+      </c>
+      <c r="B47" s="122">
+        <v>1E-3</v>
+      </c>
+      <c r="D47" s="120"/>
+      <c r="I47" s="121"/>
+      <c r="J47" s="120"/>
+      <c r="K47" s="120"/>
+      <c r="L47" s="120"/>
+      <c r="Q47" s="46"/>
+    </row>
+    <row r="48" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="130" t="s">
+        <v>153</v>
+      </c>
+      <c r="B48" s="136">
+        <v>1E-3</v>
+      </c>
+      <c r="D48" s="120"/>
+      <c r="I48" s="121"/>
+      <c r="J48" s="120"/>
+      <c r="K48" s="120"/>
+      <c r="L48" s="120"/>
+      <c r="Q48" s="46"/>
+    </row>
+    <row r="49" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="130" t="s">
+        <v>154</v>
+      </c>
+      <c r="B49" s="136">
+        <v>1E-3</v>
+      </c>
+      <c r="D49" s="120"/>
+      <c r="I49" s="121"/>
+      <c r="J49" s="120"/>
+      <c r="K49" s="120"/>
+      <c r="L49" s="120"/>
+      <c r="Q49" s="46"/>
+    </row>
+    <row r="50" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="130" t="s">
+        <v>155</v>
+      </c>
+      <c r="B50" s="136">
+        <v>9.3185000000000004E-2</v>
+      </c>
+      <c r="D50" s="120"/>
+      <c r="I50" s="121"/>
+      <c r="J50" s="120"/>
+      <c r="K50" s="120"/>
+      <c r="L50" s="120"/>
+      <c r="Q50" s="46"/>
+    </row>
+    <row r="51" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="130" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" s="136">
+        <v>1E-3</v>
+      </c>
+      <c r="D51" s="120"/>
+      <c r="I51" s="121"/>
+      <c r="J51" s="120"/>
+      <c r="K51" s="120"/>
+      <c r="L51" s="120"/>
+      <c r="Q51" s="46"/>
+    </row>
+    <row r="52" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="130" t="s">
+        <v>157</v>
+      </c>
+      <c r="B52" s="136">
+        <v>1E-3</v>
+      </c>
+      <c r="D52" s="120"/>
+      <c r="I52" s="121"/>
+      <c r="J52" s="120"/>
+      <c r="K52" s="120"/>
+      <c r="L52" s="120"/>
+      <c r="Q52" s="46"/>
+    </row>
+    <row r="53" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="130" t="s">
+        <v>158</v>
+      </c>
+      <c r="B53" s="136">
+        <v>2.7310938E-2</v>
+      </c>
+      <c r="D53" s="120"/>
+      <c r="I53" s="121"/>
+      <c r="J53" s="120"/>
+      <c r="K53" s="120"/>
+      <c r="L53" s="120"/>
+    </row>
+    <row r="54" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="130" t="s">
+        <v>159</v>
+      </c>
+      <c r="B54" s="136">
+        <v>3.3969125000000003E-2</v>
+      </c>
+      <c r="D54" s="120"/>
+      <c r="I54" s="121"/>
+      <c r="J54" s="120"/>
+      <c r="K54" s="120"/>
+      <c r="L54" s="120"/>
+    </row>
+    <row r="55" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="130" t="s">
+        <v>160</v>
+      </c>
+      <c r="B55" s="136">
+        <v>3.3969125000000003E-2</v>
+      </c>
+      <c r="D55" s="120"/>
+      <c r="I55" s="121"/>
+      <c r="J55" s="120"/>
+      <c r="K55" s="120"/>
+      <c r="L55" s="120"/>
+    </row>
+    <row r="56" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="130" t="s">
+        <v>161</v>
+      </c>
+      <c r="B56" s="136">
+        <v>3.3969125000000003E-2</v>
+      </c>
+      <c r="D56" s="120"/>
+      <c r="I56" s="121"/>
+      <c r="J56" s="120"/>
+      <c r="K56" s="120"/>
+      <c r="L56" s="120"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A57" s="131" t="s">
+        <v>162</v>
+      </c>
+      <c r="B57" s="136">
+        <v>3.3969125000000003E-2</v>
+      </c>
+      <c r="D57" s="120"/>
+      <c r="I57" s="121"/>
+      <c r="J57" s="120"/>
+      <c r="K57" s="120"/>
+      <c r="L57" s="120"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A58" s="131" t="s">
+        <v>163</v>
+      </c>
+      <c r="B58" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D58" s="120"/>
+      <c r="I58" s="121"/>
+      <c r="J58" s="120"/>
+      <c r="K58" s="120"/>
+      <c r="L58" s="120"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A59" s="132" t="s">
+        <v>164</v>
+      </c>
+      <c r="B59" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D59" s="120"/>
+      <c r="I59" s="121"/>
+      <c r="J59" s="120"/>
+      <c r="K59" s="120"/>
+      <c r="L59" s="120"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A60" s="132" t="s">
+        <v>165</v>
+      </c>
+      <c r="B60" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D60" s="120"/>
+      <c r="I60" s="121"/>
+      <c r="J60" s="120"/>
+      <c r="K60" s="120"/>
+      <c r="L60" s="120"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A61" s="131" t="s">
+        <v>166</v>
+      </c>
+      <c r="B61" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D61" s="120"/>
+      <c r="I61" s="120"/>
+      <c r="J61" s="120"/>
+      <c r="K61" s="120"/>
+      <c r="L61" s="120"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A62" s="131" t="s">
+        <v>167</v>
+      </c>
+      <c r="B62" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D62" s="120"/>
+      <c r="I62" s="120"/>
+      <c r="J62" s="120"/>
+      <c r="K62" s="120"/>
+      <c r="L62" s="120"/>
+    </row>
+    <row r="63" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="131" t="s">
+        <v>168</v>
+      </c>
+      <c r="B63" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D63" s="120"/>
+      <c r="I63" s="124"/>
+      <c r="J63" s="124"/>
+      <c r="K63" s="124"/>
+      <c r="L63" s="120"/>
+    </row>
+    <row r="64" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="131" t="s">
+        <v>169</v>
+      </c>
+      <c r="B64" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D64" s="120"/>
+      <c r="I64" s="124"/>
+      <c r="J64" s="124"/>
+      <c r="K64" s="124"/>
+      <c r="L64" s="120"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A65" s="131" t="s">
+        <v>170</v>
+      </c>
+      <c r="B65" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D65" s="120"/>
+      <c r="G65" s="120"/>
+      <c r="H65" s="120"/>
+      <c r="I65" s="120"/>
+      <c r="J65" s="120"/>
+      <c r="K65" s="120"/>
+      <c r="L65" s="120"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A66" s="131" t="s">
+        <v>171</v>
+      </c>
+      <c r="B66" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D66" s="120"/>
+      <c r="G66" s="120"/>
+      <c r="H66" s="120"/>
+      <c r="I66" s="120"/>
+      <c r="J66" s="120"/>
+      <c r="K66" s="120"/>
+      <c r="L66" s="120"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A67" s="131" t="s">
+        <v>172</v>
+      </c>
+      <c r="B67" s="136">
+        <v>1.375E-2</v>
+      </c>
+      <c r="D67" s="120"/>
+      <c r="G67" s="120"/>
+      <c r="H67" s="120"/>
+      <c r="I67" s="120"/>
+      <c r="J67" s="120"/>
+      <c r="K67" s="120"/>
+      <c r="L67" s="120"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A68" s="131" t="s">
+        <v>173</v>
+      </c>
+      <c r="B68" s="136">
+        <v>0.02</v>
+      </c>
+      <c r="D68" s="120"/>
+      <c r="G68" s="120"/>
+      <c r="H68" s="120"/>
+      <c r="I68" s="120"/>
+      <c r="J68" s="120"/>
+      <c r="K68" s="120"/>
+      <c r="L68" s="120"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A69" s="131" t="s">
+        <v>174</v>
+      </c>
+      <c r="B69" s="136">
+        <v>0.02</v>
+      </c>
+      <c r="D69" s="120"/>
+      <c r="G69" s="120"/>
+      <c r="H69" s="120"/>
+      <c r="I69" s="120"/>
+      <c r="J69" s="120"/>
+      <c r="K69" s="120"/>
+      <c r="L69" s="120"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A70" s="133" t="s">
+        <v>175</v>
+      </c>
+      <c r="B70" s="136">
+        <v>0.23300000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A71" s="133" t="s">
+        <v>176</v>
+      </c>
+      <c r="B71" s="136">
+        <v>0.28799999999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A72" s="133" t="s">
+        <v>177</v>
+      </c>
+      <c r="B72" s="136">
+        <v>0.54337400000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A73" s="133" t="s">
+        <v>178</v>
+      </c>
+      <c r="B73" s="136">
+        <v>0.1285</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A74" s="133" t="s">
+        <v>179</v>
+      </c>
+      <c r="B74" s="136">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A75" s="133" t="s">
+        <v>180</v>
+      </c>
+      <c r="B75" s="136">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A76" s="133" t="s">
+        <v>181</v>
+      </c>
+      <c r="B76" s="136">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A77" s="133" t="s">
+        <v>182</v>
+      </c>
+      <c r="B77" s="136">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A78" s="133" t="s">
+        <v>183</v>
+      </c>
+      <c r="B78" s="136">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A79" s="133" t="s">
+        <v>184</v>
+      </c>
+      <c r="B79" s="136">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A80" s="133" t="s">
+        <v>185</v>
+      </c>
+      <c r="B80" s="136">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="133" t="s">
+        <v>186</v>
+      </c>
+      <c r="B81" s="136">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="133" t="s">
+        <v>187</v>
+      </c>
+      <c r="B82" s="136">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="134" t="s">
+        <v>188</v>
+      </c>
+      <c r="B83" s="136">
+        <v>1.375E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="134" t="s">
+        <v>189</v>
+      </c>
+      <c r="B84" s="136">
+        <v>3.3969125000000003E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="134" t="s">
+        <v>190</v>
+      </c>
+      <c r="B85" s="120">
+        <v>2.0500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="134" t="s">
+        <v>191</v>
+      </c>
+      <c r="B86" s="120">
+        <v>2.0500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="134" t="s">
+        <v>192</v>
+      </c>
+      <c r="B87" s="120">
+        <v>2.0500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="134" t="s">
+        <v>193</v>
+      </c>
+      <c r="B88" s="120">
+        <v>2.0500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="134" t="s">
+        <v>194</v>
+      </c>
+      <c r="B89" s="122">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="134" t="s">
+        <v>195</v>
+      </c>
+      <c r="B90" s="136">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="135" t="s">
+        <v>196</v>
+      </c>
+      <c r="B91" s="136">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="135" t="s">
+        <v>197</v>
+      </c>
+      <c r="B92" s="136">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="135" t="s">
+        <v>198</v>
+      </c>
+      <c r="B93" s="120">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="135" t="s">
+        <v>199</v>
+      </c>
+      <c r="B94" s="120">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="135" t="s">
+        <v>200</v>
+      </c>
+      <c r="B95" s="120">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="135" t="s">
+        <v>201</v>
+      </c>
+      <c r="B96" s="120">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="135" t="s">
+        <v>202</v>
+      </c>
+      <c r="B97" s="120">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="135" t="s">
+        <v>203</v>
+      </c>
+      <c r="B98" s="120">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="135" t="s">
+        <v>204</v>
+      </c>
+      <c r="B99" s="120">
+        <v>0.105</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C6:C31">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:C52">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>0.01</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>"0..01"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>